<commit_message>
Pages:   Admin   Employees DataBaseContext:   ModifiedContext
</commit_message>
<xml_diff>
--- a/Libs/PavilionsData/Resources/Employees.xlsx
+++ b/Libs/PavilionsData/Resources/Employees.xlsx
@@ -63,9 +63,6 @@
     <t>Elizor@gmai.com</t>
   </si>
   <si>
-    <t>yntiRS#</t>
-  </si>
-  <si>
     <t>Муж</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>Статус записи</t>
+  </si>
+  <si>
+    <t>ynt1RS#</t>
   </si>
 </sst>
 </file>
@@ -577,7 +577,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +626,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="G2" s="1">
         <v>4</v>
@@ -655,7 +655,7 @@
         <v>71070628291</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -663,19 +663,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G3" s="1">
         <v>2</v>
@@ -684,7 +684,7 @@
         <v>73341460151</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -692,19 +692,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="G4" s="1">
         <v>3</v>
@@ -713,7 +713,7 @@
         <v>78560519329</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -721,19 +721,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
@@ -742,7 +742,7 @@
         <v>78248932403</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -750,19 +750,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="G6" s="1">
         <v>4</v>
@@ -771,7 +771,7 @@
         <v>76402701310</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -779,19 +779,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="G7" s="1">
         <v>4</v>
@@ -800,7 +800,7 @@
         <v>79292074471</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -808,19 +808,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="G8" s="1">
         <v>2</v>
@@ -829,7 +829,7 @@
         <v>74050887389</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -837,19 +837,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>48</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="G9" s="1">
         <v>4</v>
@@ -858,7 +858,7 @@
         <v>76010195020</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -866,19 +866,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
         <v>52</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>53</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="G10" s="1">
         <v>3</v>
@@ -887,7 +887,7 @@
         <v>70784295786</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -895,19 +895,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
         <v>57</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>58</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
@@ -916,7 +916,7 @@
         <v>76394904016</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -924,19 +924,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>63</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="G12" s="1">
         <v>2</v>
@@ -945,7 +945,7 @@
         <v>72232649591</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -953,19 +953,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
         <v>67</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>68</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="G13" s="1">
         <v>3</v>
@@ -974,7 +974,7 @@
         <v>77897623028</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>